<commit_message>
Add feature to handle multiple student's result and save the output as file
</commit_message>
<xml_diff>
--- a/csv/student_course_result.xlsx
+++ b/csv/student_course_result.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idecupm-my.sharepoint.com/personal/206730_student_upm_edu_my/Documents/UPM Sem 7/ECC4208 Advanced Programming/Assignment/CalculateCGPA/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28065992-4290-4078-9A41-33C279B13366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{28065992-4290-4078-9A41-33C279B13366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33EE85A8-A15E-49CA-AAFE-BD0CE614A3C4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student_course_result" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,8 +511,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -556,6 +570,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -854,160 +872,218 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="B1">
-        <v>2.38</v>
-      </c>
-      <c r="C1">
-        <v>2.57</v>
-      </c>
-      <c r="D1">
-        <v>3.21</v>
-      </c>
-      <c r="E1">
-        <v>3.34</v>
-      </c>
-      <c r="F1">
-        <v>2.44</v>
-      </c>
-      <c r="G1">
-        <v>2.2999999999999998</v>
+      <c r="A1" s="1">
+        <f ca="1">RAND() * 2 + 2</f>
+        <v>3.7467381498672854</v>
+      </c>
+      <c r="B1" s="1">
+        <f t="shared" ref="B1:G8" ca="1" si="0">RAND() * 2 + 2</f>
+        <v>3.7569673304686364</v>
+      </c>
+      <c r="C1" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9035227985709398</v>
+      </c>
+      <c r="D1" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7478348036128351</v>
+      </c>
+      <c r="E1" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5947674127501958</v>
+      </c>
+      <c r="F1" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9872336377530146</v>
+      </c>
+      <c r="G1" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4320781689066706</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3.82</v>
-      </c>
-      <c r="B2">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="C2">
-        <v>2.81</v>
-      </c>
-      <c r="D2">
-        <v>3.48</v>
-      </c>
-      <c r="E2">
-        <v>3.84</v>
-      </c>
-      <c r="F2">
-        <v>2.75</v>
-      </c>
+      <c r="A2" s="1">
+        <f ca="1">RAND() * 2 + 2</f>
+        <v>2.2853254264811378</v>
+      </c>
+      <c r="B2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.991014595179478</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.0504320625628436</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7118701576124913</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.0749442676058178</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4093244102321734</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3.8</v>
-      </c>
-      <c r="B3">
-        <v>3.1</v>
-      </c>
-      <c r="C3">
-        <v>2.31</v>
-      </c>
-      <c r="D3">
-        <v>3.67</v>
-      </c>
-      <c r="E3">
-        <v>2.15</v>
-      </c>
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A8" ca="1" si="1">RAND() * 2 + 2</f>
+        <v>3.7445718896729954</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4444738449034284</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.256444824836799</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1169829868193739</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2758876580901868</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3.99</v>
-      </c>
-      <c r="B4">
-        <v>3.66</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3.77</v>
-      </c>
-      <c r="E4">
-        <v>2.5499999999999998</v>
-      </c>
+      <c r="A4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.385057168557998</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.8281402212890869</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.3973768737646832</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9390551301801917</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.532761115462197</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3.4</v>
-      </c>
-      <c r="B5">
-        <v>3.05</v>
-      </c>
-      <c r="C5">
-        <v>2.46</v>
-      </c>
-      <c r="D5">
-        <v>3.32</v>
-      </c>
-      <c r="E5">
-        <v>3.45</v>
-      </c>
+      <c r="A5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.2579379009112257</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9795356738117702</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.5047899184190854</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4680625778402048</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5636382508149227</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2.48</v>
-      </c>
-      <c r="B6">
-        <v>3.65</v>
-      </c>
-      <c r="C6">
-        <v>3.84</v>
-      </c>
-      <c r="D6">
-        <v>3.54</v>
-      </c>
-      <c r="E6">
-        <v>3.9</v>
-      </c>
-      <c r="F6">
-        <v>3.66</v>
-      </c>
+      <c r="A6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6176289123962135</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9949614036540542</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7419989082233207</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.7430949145461572</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4214669505252497</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2855762224857292</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2.93</v>
-      </c>
-      <c r="B7">
-        <v>3.7</v>
-      </c>
-      <c r="C7">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="D7">
-        <v>2.44</v>
-      </c>
-      <c r="E7">
-        <v>3.64</v>
-      </c>
-      <c r="F7">
-        <v>2.94</v>
-      </c>
+      <c r="A7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.0632160866741196</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2966237999559493</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.7537975373851196</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2415149014930038</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.954137273591245</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.3845878199481874</v>
+      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3.66</v>
-      </c>
-      <c r="B8">
-        <v>2.83</v>
-      </c>
-      <c r="C8">
-        <v>2.46</v>
-      </c>
-      <c r="D8">
-        <v>3.34</v>
-      </c>
+      <c r="A8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9371330821036481</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.82859953401762</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4684138329044334</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6249878704274234</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactoring the function for parser
</commit_message>
<xml_diff>
--- a/csv/student_course_result.xlsx
+++ b/csv/student_course_result.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idecupm-my.sharepoint.com/personal/206730_student_upm_edu_my/Documents/UPM Sem 7/ECC4208 Advanced Programming/Assignment/CalculateCGPA/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{28065992-4290-4078-9A41-33C279B13366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33EE85A8-A15E-49CA-AAFE-BD0CE614A3C4}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{28065992-4290-4078-9A41-33C279B13366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CD362B1-35D8-4D6A-A84B-63F32BC026C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student_course_result" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +33,33 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -511,9 +537,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -876,214 +903,284 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <f ca="1">RAND() * 2 + 2</f>
-        <v>3.7467381498672854</v>
-      </c>
-      <c r="B1" s="1">
-        <f t="shared" ref="B1:G8" ca="1" si="0">RAND() * 2 + 2</f>
-        <v>3.7569673304686364</v>
-      </c>
-      <c r="C1" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9035227985709398</v>
-      </c>
-      <c r="D1" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7478348036128351</v>
-      </c>
-      <c r="E1" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.5947674127501958</v>
-      </c>
-      <c r="F1" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9872336377530146</v>
-      </c>
-      <c r="G1" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4320781689066706</v>
+      <c r="A1" s="1" cm="1">
+        <f t="array" aca="1" ref="A1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" cm="1">
+        <f t="array" aca="1" ref="B1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" cm="1">
+        <f t="array" aca="1" ref="C1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" cm="1">
+        <f t="array" aca="1" ref="D1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="E1" s="1" cm="1">
+        <f t="array" aca="1" ref="E1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" cm="1">
+        <f t="array" aca="1" ref="F1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" cm="1">
+        <f t="array" aca="1" ref="G1" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <f ca="1">RAND() * 2 + 2</f>
-        <v>2.2853254264811378</v>
-      </c>
-      <c r="B2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.991014595179478</v>
-      </c>
-      <c r="C2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.0504320625628436</v>
-      </c>
-      <c r="D2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7118701576124913</v>
-      </c>
-      <c r="E2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.0749442676058178</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.4093244102321734</v>
+      <c r="A2" s="1" cm="1">
+        <f t="array" aca="1" ref="A2" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="B2" s="1" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
+      </c>
+      <c r="C2" s="1" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
+      </c>
+      <c r="D2" s="1" cm="1">
+        <f t="array" aca="1" ref="D2" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="1" cm="1">
+        <f t="array" aca="1" ref="E2" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.5</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <f t="shared" ref="A3:A8" ca="1" si="1">RAND() * 2 + 2</f>
-        <v>3.7445718896729954</v>
-      </c>
-      <c r="B3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4444738449034284</v>
-      </c>
-      <c r="C3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.256444824836799</v>
-      </c>
-      <c r="D3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1169829868193739</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2758876580901868</v>
+      <c r="A3" s="1" cm="1">
+        <f t="array" aca="1" ref="A3" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.75</v>
+      </c>
+      <c r="B3" s="1" cm="1">
+        <f t="array" aca="1" ref="B3" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.5</v>
+      </c>
+      <c r="E3" s="1" cm="1">
+        <f t="array" aca="1" ref="E3" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.75</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.385057168557998</v>
-      </c>
-      <c r="B4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.8281402212890869</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.3973768737646832</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9390551301801917</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.532761115462197</v>
+      <c r="A4" s="1" cm="1">
+        <f t="array" aca="1" ref="A4" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="B4" s="1" cm="1">
+        <f t="array" aca="1" ref="B4" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.75</v>
+      </c>
+      <c r="D4" s="1" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="E4" s="1" cm="1">
+        <f t="array" aca="1" ref="E4" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.2579379009112257</v>
-      </c>
-      <c r="B5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9795356738117702</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.5047899184190854</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.4680625778402048</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.5636382508149227</v>
+      <c r="A5" s="1" cm="1">
+        <f t="array" aca="1" ref="A5" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" cm="1">
+        <f t="array" aca="1" ref="B5" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="1" cm="1">
+        <f t="array" aca="1" ref="C5" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="D5" s="1" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" cm="1">
+        <f t="array" aca="1" ref="E5" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.6176289123962135</v>
-      </c>
-      <c r="B6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9949614036540542</v>
-      </c>
-      <c r="C6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7419989082233207</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7430949145461572</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4214669505252497</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2855762224857292</v>
+      <c r="A6" s="1" cm="1">
+        <f t="array" aca="1" ref="A6" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.5</v>
+      </c>
+      <c r="B6" s="1" cm="1">
+        <f t="array" aca="1" ref="B6" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
+      </c>
+      <c r="C6" s="1" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.75</v>
+      </c>
+      <c r="D6" s="1" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="1" cm="1">
+        <f t="array" aca="1" ref="E6" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.5</v>
+      </c>
+      <c r="F6" s="1" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.5</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.0632160866741196</v>
-      </c>
-      <c r="B7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2966237999559493</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7537975373851196</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.2415149014930038</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.954137273591245</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.3845878199481874</v>
+      <c r="A7" s="1" cm="1">
+        <f t="array" aca="1" ref="A7" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="B7" s="1" cm="1">
+        <f t="array" aca="1" ref="B7" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.75</v>
+      </c>
+      <c r="C7" s="1" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="1" cm="1">
+        <f t="array" aca="1" ref="D7" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" cm="1">
+        <f t="array" aca="1" ref="E7" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
+      </c>
+      <c r="F7" s="1" cm="1">
+        <f t="array" aca="1" ref="F7" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.9371330821036481</v>
-      </c>
-      <c r="B8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.82859953401762</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4684138329044334</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.6249878704274234</v>
+      <c r="A8" s="1" cm="1">
+        <f t="array" aca="1" ref="A8" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.75</v>
+      </c>
+      <c r="B8" s="1" cm="1">
+        <f t="array" aca="1" ref="B8" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>1.75</v>
+      </c>
+      <c r="C8" s="1" cm="1">
+        <f t="array" aca="1" ref="C8" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="1" cm="1">
+        <f t="array" aca="1" ref="D8" ca="1">INDEX({4,3.75,3.5,3,2.75,2.5,2,1.75,1.5,1}, RANDBETWEEN(1, 10))</f>
+        <v>2.75</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE36BCC-3B02-4489-8187-14FDD983F012}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>